<commit_message>
Added basic functionality needed to create new files from an existing excel file
</commit_message>
<xml_diff>
--- a/src/Extension.OfficeOpemXml.Tests/Resources/Beispieltabelle.xlsx
+++ b/src/Extension.OfficeOpemXml.Tests/Resources/Beispieltabelle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\C#\Extension.OfficeOpenXml\src\Extension.OfficeOpemXml.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C0F67F-E811-488E-83B4-E4861AC02635}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D170DA8-65AA-4C73-BBE2-68139A2140B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -660,7 +660,7 @@
   <cols>
     <col min="1" max="1" width="11.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="7" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="5.85546875" style="2" customWidth="1"/>

</xml_diff>

<commit_message>
Get column index and copy cell formula
</commit_message>
<xml_diff>
--- a/src/Extension.OfficeOpemXml.Tests/Resources/Beispieltabelle.xlsx
+++ b/src/Extension.OfficeOpemXml.Tests/Resources/Beispieltabelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\C#\Extension.OfficeOpenXml\src\Extension.OfficeOpemXml.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D170DA8-65AA-4C73-BBE2-68139A2140B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F120664E-096B-454C-A463-2C4C7E42A0A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorgangsuebersicht" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>Angebotsnummer</t>
   </si>
@@ -124,12 +124,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>xx</t>
-  </si>
-  <si>
     <t>AAA</t>
   </si>
   <si>
@@ -141,12 +135,48 @@
   <si>
     <t>DDD</t>
   </si>
+  <si>
+    <t>A012020</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>24243,00</t>
+  </si>
+  <si>
+    <t>24243,08</t>
+  </si>
+  <si>
+    <t>24243,07</t>
+  </si>
+  <si>
+    <t>24243,06</t>
+  </si>
+  <si>
+    <t>24243,05</t>
+  </si>
+  <si>
+    <t>24243,04</t>
+  </si>
+  <si>
+    <t>24243,03</t>
+  </si>
+  <si>
+    <t>24243,02</t>
+  </si>
+  <si>
+    <t>24243,01</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="9.5"/>
       <name val="Arial"/>
@@ -202,6 +232,12 @@
     </font>
     <font>
       <sz val="9.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -317,13 +353,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="3" xfId="3"/>
+    <xf numFmtId="3" fontId="6" fillId="6" borderId="3" xfId="2"/>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Ausgabe" xfId="8" builtinId="21" customBuiltin="1"/>
@@ -653,13 +692,13 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P484" sqref="P484"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="54.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" style="2" customWidth="1"/>
@@ -678,19 +717,19 @@
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F1"/>
       <c r="G1"/>
@@ -718,8 +757,8 @@
       <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>33</v>
+      <c r="E2" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
@@ -747,8 +786,8 @@
       <c r="D3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>33</v>
+      <c r="E3" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
@@ -776,8 +815,8 @@
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>33</v>
+      <c r="E4" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="F4"/>
       <c r="G4"/>
@@ -805,8 +844,8 @@
       <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
+      <c r="E5" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
@@ -834,8 +873,8 @@
       <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>33</v>
+      <c r="E6" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="F6"/>
       <c r="G6"/>
@@ -863,8 +902,8 @@
       <c r="D7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>33</v>
+      <c r="E7" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
@@ -892,8 +931,8 @@
       <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>33</v>
+      <c r="E8" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
@@ -921,7 +960,9 @@
       <c r="D9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="F9"/>
       <c r="G9"/>
       <c r="H9"/>
@@ -948,8 +989,8 @@
       <c r="D10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>33</v>
+      <c r="E10" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -977,8 +1018,8 @@
       <c r="D11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>33</v>
+      <c r="E11" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
@@ -1006,8 +1047,8 @@
       <c r="D12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>33</v>
+      <c r="E12" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
@@ -1035,7 +1076,9 @@
       <c r="D13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13"/>
@@ -1062,8 +1105,8 @@
       <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>33</v>
+      <c r="E14" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -1079,23 +1122,33 @@
       <c r="Q14"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
+      <c r="A15" s="4">
+        <v>61160633</v>
+      </c>
+      <c r="B15" s="4">
+        <v>125843</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16"/>
@@ -10222,7 +10275,8 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q2498">
     <sortCondition ref="A2:A2498"/>
   </sortState>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="75" orientation="landscape"/>
+  <pageSetup scale="75" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made use of shared strings to correctly display formatting
</commit_message>
<xml_diff>
--- a/src/Extension.OfficeOpemXml.Tests/Resources/Beispieltabelle.xlsx
+++ b/src/Extension.OfficeOpemXml.Tests/Resources/Beispieltabelle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\C#\Extension.OfficeOpenXml\src\Extension.OfficeOpemXml.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F120664E-096B-454C-A463-2C4C7E42A0A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4467F4E1-E14A-4110-91EF-C04721C9A472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,69 +23,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Angebotsnummer</t>
-  </si>
-  <si>
-    <t>12345</t>
-  </si>
-  <si>
-    <t>12346</t>
-  </si>
-  <si>
-    <t>12347</t>
-  </si>
-  <si>
-    <t>12348</t>
-  </si>
-  <si>
-    <t>12349</t>
-  </si>
-  <si>
-    <t>13456</t>
-  </si>
-  <si>
-    <t>13457</t>
-  </si>
-  <si>
-    <t>13458</t>
-  </si>
-  <si>
-    <t>12457</t>
-  </si>
-  <si>
-    <t>23456</t>
-  </si>
-  <si>
-    <t>45667</t>
-  </si>
-  <si>
-    <t>56789</t>
-  </si>
-  <si>
-    <t>45678</t>
   </si>
   <si>
     <t>a</t>
   </si>
   <si>
     <t>d</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>sdf</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>gf</t>
   </si>
   <si>
     <t>xxxxxxxx</t>
@@ -115,58 +61,67 @@
     <t>edddddd</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>AAA</t>
-  </si>
-  <si>
-    <t>BBB</t>
-  </si>
-  <si>
-    <t>CCC</t>
-  </si>
-  <si>
-    <t>DDD</t>
-  </si>
-  <si>
     <t>A012020</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>12.08.2020</t>
   </si>
   <si>
-    <t>24243,00</t>
+    <t>12.08.2021</t>
   </si>
   <si>
-    <t>24243,08</t>
+    <t>12.08.2022</t>
   </si>
   <si>
-    <t>24243,07</t>
+    <t>12.08.2023</t>
   </si>
   <si>
-    <t>24243,06</t>
+    <t>12.08.2024</t>
   </si>
   <si>
-    <t>24243,05</t>
+    <t>12.08.2025</t>
   </si>
   <si>
-    <t>24243,04</t>
+    <t>12.08.2026</t>
   </si>
   <si>
-    <t>24243,03</t>
+    <t>12.08.2027</t>
   </si>
   <si>
-    <t>24243,02</t>
+    <t>12.08.2028</t>
   </si>
   <si>
-    <t>24243,01</t>
+    <t>12.08.2029</t>
+  </si>
+  <si>
+    <t>12.08.2030</t>
+  </si>
+  <si>
+    <t>12.08.2031</t>
+  </si>
+  <si>
+    <t>12.08.2032</t>
+  </si>
+  <si>
+    <t>12.08.2033</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Another Format</t>
   </si>
 </sst>
 </file>
@@ -176,7 +131,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="9.5"/>
       <name val="Arial"/>
@@ -242,8 +197,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF003C65"/>
+      <name val="Avenir Next LT Pro"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +242,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF73B1DD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,7 +322,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -363,6 +332,9 @@
     <xf numFmtId="49" fontId="6" fillId="6" borderId="3" xfId="3"/>
     <xf numFmtId="3" fontId="6" fillId="6" borderId="3" xfId="2"/>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Ausgabe" xfId="8" builtinId="21" customBuiltin="1"/>
@@ -690,9 +662,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q495"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -701,7 +673,7 @@
     <col min="2" max="2" width="16.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="54.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="75.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="5.85546875" style="2" customWidth="1"/>
     <col min="7" max="8" width="7" style="2" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" style="2" customWidth="1"/>
@@ -717,19 +689,19 @@
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F1"/>
       <c r="G1"/>
@@ -744,21 +716,21 @@
       <c r="P1"/>
       <c r="Q1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
+      <c r="D2" s="9">
+        <v>0.152</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>40</v>
+      <c r="E2" s="6">
+        <v>2424302</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
@@ -773,21 +745,21 @@
       <c r="P2"/>
       <c r="Q2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
+      <c r="C3" s="8" t="s">
+        <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>30</v>
+      <c r="D3" s="9">
+        <v>0.152</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>41</v>
+      <c r="E3" s="6">
+        <v>2424302</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
@@ -802,21 +774,21 @@
       <c r="P3"/>
       <c r="Q3"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
+      <c r="C4" s="8" t="s">
+        <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>31</v>
+      <c r="D4" s="9">
+        <v>0.152</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>42</v>
+      <c r="E4" s="6">
+        <v>2424302</v>
       </c>
       <c r="F4"/>
       <c r="G4"/>
@@ -831,21 +803,21 @@
       <c r="P4"/>
       <c r="Q4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
+      <c r="C5" s="8" t="s">
+        <v>6</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
+      <c r="D5" s="9">
+        <v>0.152</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>43</v>
+      <c r="E5" s="6">
+        <v>2424302</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
@@ -860,21 +832,21 @@
       <c r="P5"/>
       <c r="Q5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
+      <c r="C6" s="8" t="s">
+        <v>7</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>32</v>
+      <c r="D6" s="9">
+        <v>0.152</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>44</v>
+      <c r="E6" s="6">
+        <v>2424302</v>
       </c>
       <c r="F6"/>
       <c r="G6"/>
@@ -889,21 +861,21 @@
       <c r="P6"/>
       <c r="Q6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
+      <c r="C7" s="8" t="s">
+        <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
+      <c r="D7" s="9">
+        <v>0.152</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>45</v>
+      <c r="E7" s="6">
+        <v>2424302</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
@@ -918,21 +890,21 @@
       <c r="P7"/>
       <c r="Q7"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
+    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>27</v>
+      <c r="C8" s="8" t="s">
+        <v>9</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
+      <c r="D8" s="9">
+        <v>0.152</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>46</v>
+      <c r="E8" s="6">
+        <v>2424302</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
@@ -947,21 +919,21 @@
       <c r="P8"/>
       <c r="Q8"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
+    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>30</v>
+      <c r="D9" s="9">
+        <v>0.152</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>47</v>
+      <c r="E9" s="6">
+        <v>2424302</v>
       </c>
       <c r="F9"/>
       <c r="G9"/>
@@ -976,21 +948,21 @@
       <c r="P9"/>
       <c r="Q9"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
+      <c r="D10" s="9">
+        <v>0.152</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>39</v>
+      <c r="E10" s="6">
+        <v>2424302</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -1005,21 +977,21 @@
       <c r="P10"/>
       <c r="Q10"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
+    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>30</v>
+      <c r="D11" s="9">
+        <v>0.152</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>47</v>
+      <c r="E11" s="6">
+        <v>2424302</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
@@ -1034,21 +1006,21 @@
       <c r="P11"/>
       <c r="Q11"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
+    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>32</v>
+      <c r="D12" s="9">
+        <v>0.152</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>46</v>
+      <c r="E12" s="6">
+        <v>2424302</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
@@ -1063,21 +1035,21 @@
       <c r="P12"/>
       <c r="Q12"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
+    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>31</v>
+      <c r="D13" s="9">
+        <v>0.152</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>45</v>
+      <c r="E13" s="6">
+        <v>2424302</v>
       </c>
       <c r="F13"/>
       <c r="G13"/>
@@ -1092,21 +1064,21 @@
       <c r="P13"/>
       <c r="Q13"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
+    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>32</v>
+      <c r="D14" s="9">
+        <v>0.152</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>44</v>
+      <c r="E14" s="6">
+        <v>2424302</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -1121,21 +1093,21 @@
       <c r="P14"/>
       <c r="Q14"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
-        <v>61160633</v>
+    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>26</v>
       </c>
-      <c r="B15" s="4">
-        <v>125843</v>
+      <c r="B15" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>38</v>
+      <c r="D15" s="9">
+        <v>0.152</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>43</v>
+      <c r="E15" s="6">
+        <v>2424302</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>

</xml_diff>

<commit_message>
Also copy cell formulas
</commit_message>
<xml_diff>
--- a/src/Extension.OfficeOpemXml.Tests/Resources/Beispieltabelle.xlsx
+++ b/src/Extension.OfficeOpemXml.Tests/Resources/Beispieltabelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\C#\Extension.OfficeOpenXml\src\Extension.OfficeOpemXml.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4467F4E1-E14A-4110-91EF-C04721C9A472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DA490A-F8CD-4BBD-9D15-061949BCA750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorgangsuebersicht" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Vorgangsuebersicht!$A$1:$Q$493</definedName>
   </definedNames>
-  <calcPr calcId="162913" fullPrecision="0"/>
+  <calcPr calcId="191029" fullPrecision="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -322,7 +332,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -335,6 +345,7 @@
     <xf numFmtId="14" fontId="6" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="8" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="10" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Ausgabe" xfId="8" builtinId="21" customBuiltin="1"/>
@@ -662,9 +673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q495"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -716,7 +727,7 @@
       <c r="P1"/>
       <c r="Q1"/>
     </row>
-    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
@@ -1127,7 +1138,10 @@
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
-      <c r="E16"/>
+      <c r="E16" s="10">
+        <f>SUM(E2:E15)</f>
+        <v>33940228</v>
+      </c>
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>

</xml_diff>

<commit_message>
Fix for empty cells
</commit_message>
<xml_diff>
--- a/src/Extension.OfficeOpemXml.Tests/Resources/Beispieltabelle.xlsx
+++ b/src/Extension.OfficeOpemXml.Tests/Resources/Beispieltabelle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\C#\Extension.OfficeOpenXml\src\Extension.OfficeOpemXml.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DA490A-F8CD-4BBD-9D15-061949BCA750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2735421C-D7D1-4B59-AE0C-BB07BE292411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Vorgangsuebersicht" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Vorgangsuebersicht!$A$1:$Q$493</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Vorgangsuebersicht!$A$2:$Q$494</definedName>
   </definedNames>
   <calcPr calcId="191029" fullPrecision="0"/>
   <extLst>
@@ -332,7 +332,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -346,6 +346,7 @@
     <xf numFmtId="49" fontId="6" fillId="8" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="10" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Ausgabe" xfId="8" builtinId="21" customBuiltin="1"/>
@@ -671,11 +672,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q495"/>
+  <dimension ref="A1:Q496"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -698,50 +699,27 @@
     <col min="17" max="17" width="9.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E1" s="11">
+        <f>SUM(E3:E16)</f>
+        <v>33940228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1"/>
-      <c r="O1"/>
-      <c r="P1"/>
-      <c r="Q1"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0.152</v>
-      </c>
-      <c r="E2" s="6">
-        <v>2424302</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
@@ -758,13 +736,13 @@
     </row>
     <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>4</v>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="D3" s="9">
         <v>0.152</v>
@@ -787,13 +765,13 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="9">
         <v>0.152</v>
@@ -816,13 +794,13 @@
     </row>
     <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="9">
         <v>0.152</v>
@@ -845,13 +823,13 @@
     </row>
     <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="9">
         <v>0.152</v>
@@ -874,13 +852,13 @@
     </row>
     <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="9">
         <v>0.152</v>
@@ -903,13 +881,13 @@
     </row>
     <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="9">
         <v>0.152</v>
@@ -932,13 +910,13 @@
     </row>
     <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
+      <c r="C9" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="D9" s="9">
         <v>0.152</v>
@@ -961,13 +939,13 @@
     </row>
     <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="9">
         <v>0.152</v>
@@ -990,13 +968,13 @@
     </row>
     <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="9">
         <v>0.152</v>
@@ -1019,13 +997,13 @@
     </row>
     <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12" s="9">
         <v>0.152</v>
@@ -1048,13 +1026,13 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13" s="9">
         <v>0.152</v>
@@ -1077,13 +1055,13 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D14" s="9">
         <v>0.152</v>
@@ -1106,13 +1084,13 @@
     </row>
     <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>12</v>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D15" s="9">
         <v>0.152</v>
@@ -1120,47 +1098,54 @@
       <c r="E15" s="6">
         <v>2424302</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16" s="10">
-        <f>SUM(E2:E15)</f>
-        <v>33940228</v>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>26</v>
       </c>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16"/>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.152</v>
+      </c>
+      <c r="E16" s="6">
+        <v>2424302</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
-      <c r="E17"/>
+      <c r="E17" s="10"/>
       <c r="F17"/>
       <c r="G17"/>
       <c r="H17"/>
@@ -10256,10 +10241,29 @@
       <c r="P495"/>
       <c r="Q495"/>
     </row>
+    <row r="496" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A496"/>
+      <c r="B496"/>
+      <c r="C496"/>
+      <c r="D496"/>
+      <c r="E496"/>
+      <c r="F496"/>
+      <c r="G496"/>
+      <c r="H496"/>
+      <c r="I496"/>
+      <c r="J496"/>
+      <c r="K496"/>
+      <c r="L496"/>
+      <c r="M496"/>
+      <c r="N496"/>
+      <c r="O496"/>
+      <c r="P496"/>
+      <c r="Q496"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q493" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q2498">
-    <sortCondition ref="A2:A2498"/>
+  <autoFilter ref="A2:Q494" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Q2499">
+    <sortCondition ref="A3:A2499"/>
   </sortState>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>